<commit_message>
add important notes and last updated dates
</commit_message>
<xml_diff>
--- a/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvIncidentes.xlsx
+++ b/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvIncidentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixbaez822/Desktop/ViolenciaGeneroPR/data/Sistema_de_Notificacion_de_Muertes_Violentas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Sistema_de_Notificacion_de_Muertes_Violentas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3701DEFF-AA61-6D4A-AA04-A122CA6DA955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D100FBF9-6D5B-4478-959A-6F1E3593EA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16320" xr2:uid="{9CFC54A2-FB65-C045-ACC9-D5EBAFBDCE35}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9CFC54A2-FB65-C045-ACC9-D5EBAFBDCE35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,9 +430,12 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="53.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -478,7 +481,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -501,7 +504,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -524,7 +527,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -547,7 +550,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -570,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -593,7 +596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -616,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -639,7 +642,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
modify empty plot message size to be responsive, modify years in OPM line plot and change facets in Correccion and Dept. Familia
</commit_message>
<xml_diff>
--- a/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvIncidentes.xlsx
+++ b/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvIncidentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Sistema_de_Notificacion_de_Muertes_Violentas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B10DD25-D337-40FF-B159-DBD35323BE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9D469A8-A514-4FC1-B83D-F7B274420B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9CFC54A2-FB65-C045-ACC9-D5EBAFBDCE35}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>Homicidio seguido de suicidio</t>
   </si>
   <si>
-    <t>Homicidio(s) seguido de suicidio(s), (más  de dos víctimas)</t>
+    <t>Homicidio(s) seguido de suicidio(s), (+ dos víctimas)</t>
   </si>
   <si>
     <t>Muerte no determinada</t>
@@ -435,7 +435,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>

</xml_diff>